<commit_message>
Test cases according to Phase 4 & phase 5
</commit_message>
<xml_diff>
--- a/Tests/Project Test Cases.xlsx
+++ b/Tests/Project Test Cases.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>Functionality</t>
   </si>
@@ -108,12 +108,148 @@
   <si>
     <t>Atech Computers Website Test Cases</t>
   </si>
+  <si>
+    <t>1) Sign in as the administrator;</t>
+  </si>
+  <si>
+    <t>1) Choose file and choose appropriate provider and press"Import".
+2) Choose file and choose appropriate provider without pressing "Import" button.</t>
+  </si>
+  <si>
+    <t>1) Observe the page below, it will shows number of products in a choosen provider file. For example : you have choosen PB as provider and choose its matching file and press import. It will shows "You are going to import 40 products".
+2) It will shows that "You are going to import 0 products"</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>1) Go to the address bar of your browser and type website address, press enter
+2) Observe the new page.</t>
+  </si>
+  <si>
+    <t>1) Go to "Home Page" by default.
+2) Page layout is correct: no component is missing or is in a wrong position; all buttons are working.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Verify the header and footer
+2) Verify the title of Home Page
+3) Verify slideshow of images in Home page
+</t>
+  </si>
+  <si>
+    <t>1) Menubar and title is in header and in footer it is written"Copyright Atech Computers, 2016. All rights reserved" 
+2) Welcome: IBUTIT with cool images.
+3) Images should switch automatically in set time period.</t>
+  </si>
+  <si>
+    <t>1) Verify the Home link on top left side of Menu bar
+2) Verify the Product page link located in menubar of Home page.
+3) Verify the About Us link located in menubar of home page
+4) Verify the sign-in box located on top right corner of home page.</t>
+  </si>
+  <si>
+    <t>1) It will direct the user to the actual Home page.
+2) It will direct the user to the Product page.
+3) It will direct the user to the About Us page
+4) It will allow user to sign-in as user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Verify link of Cart located on top right corner of website.
+2) Click on Cart icon located on top right corner on Home page without adding any product to cart.
+3) Click on Cart located on top right corner in home page after adding product to cart.
+4) After adding products to Cart and you want to add another product to then click on "Keep on Shopping".
+5) To see product list added into the Cart, click Cart icon located on top right corner to the Home page.
+</t>
+  </si>
+  <si>
+    <t>1) It will direct the user to the Cart page.
+2) It will go to Cart page and show message "We're Sad. Your cart is empty".
+3) It will go to Cart page and show number of products added by user into Cart.
+4) It will go to Product page again to allow the user to select another product.
+5) It will show details of products on the side of Cart icon.</t>
+  </si>
+  <si>
+    <t>1) Verify Categories link on home page located below menubar
+2) Click any category option listed under Categories link.</t>
+  </si>
+  <si>
+    <t>1) It will direct the user to the Product Search page.
+2) It will go to Product Search page to search that particular category.</t>
+  </si>
+  <si>
+    <t>1) Verify different brands links located unders Brands icon on Home page.</t>
+  </si>
+  <si>
+    <t>1) It will direct the user to the Product Search page to select that particular brand.</t>
+  </si>
+  <si>
+    <t>Product Page</t>
+  </si>
+  <si>
+    <t>1) Type website address in browser address bar and click on Product option in menubar located on top of the website.
+2) Observe the product page.</t>
+  </si>
+  <si>
+    <t>1) Go to the Product page.
+2) Layout is correct. No components are missing, all buttons are working correct. It includes table which contains list of Brand, Name, Retail price, and Stock colomns.</t>
+  </si>
+  <si>
+    <t>1) Click on "Search" button without selecting any brand, category or provider.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) It will show a list of all products in database.
+</t>
+  </si>
+  <si>
+    <t>1) Select any Brand from dropdown list and click search button without selecting any provider or category.
+2) Select any "Category" from dropdown list under Category and click on search without selecting any provider and brand.
+3) click any "Provider" from dropdown list under provider and click on search without selecting any brand and category.
+4) Select any brand, category and provider together and click search button.</t>
+  </si>
+  <si>
+    <t>1) It will show a list of all products from selected "Brand" located below search button.
+2) It will show a list of all products from selected "Category" located below search button from search products page.
+3) It will show a list of all products from selected "Provider" located below search button from search products page.
+4) Change to "a list of products which meet all the keywords is shown.</t>
+  </si>
+  <si>
+    <t>1) Click reset button to reset selection to its default value and then click on any link from the list under "Brand" colomn.
+2) Click reset button to reset selection to its default value and click on any link from the list under "Name" colomn.
+3) Click "Reset" button after selecting any brand, provider, and category.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1) It will show all products list related to particular selected "Brand" and it also set particular selected brand name from "Brands" drop down list.
+2) It will allow you to go to "Product details" page.
+3) It will reset all selections to its their default values.</t>
+  </si>
+  <si>
+    <t>1) Click any link from "Name" colomn.
+2) Click "Add to cart" button located below product details.
+3) Click "Back" button located below product details.</t>
+  </si>
+  <si>
+    <t>1) This page shows product details which include description, brand, stock, product no., and retail price. Layout is correct and all buttons are working correct.
+2) It will allow you to add product to cart.
+3) It will go back to Product page.</t>
+  </si>
+  <si>
+    <t>About Us</t>
+  </si>
+  <si>
+    <t>1) Verify the About Us link located on top rightside of menubar on Home page.
+2) Obeserve the About Us page.</t>
+  </si>
+  <si>
+    <t>1) It will direct the user to the About Us page
+2) Layout is correct, No components are missing. Page includes contact information, Address information, short outline of the company, Payment account details.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +285,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -158,7 +306,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -433,15 +581,149 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -457,71 +739,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,6 +917,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -651,6 +969,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -827,9 +1162,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I12"/>
+  <dimension ref="A3:I25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -843,39 +1180,39 @@
     <col min="9" max="9" width="42.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -901,121 +1238,328 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="8">
+      <c r="C7" s="18"/>
+      <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="2:9" ht="129" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="11">
+      <c r="H7" s="4"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="16"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="6">
         <v>2</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="11">
+      <c r="H8" s="7"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="16"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="6">
         <v>3</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="11">
+      <c r="H9" s="7"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="6">
         <v>4</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="2:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="11">
+      <c r="H10" s="7"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="6">
         <v>5</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="13"/>
-    </row>
-    <row r="12" spans="2:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="14">
+      <c r="H11" s="7"/>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="29">
         <v>6</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="16"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" s="31"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="9">
+        <v>7</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="35">
+        <v>8</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="6">
+        <v>9</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="6">
+        <v>10</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="6">
+        <v>11</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="6">
+        <v>12</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="9">
+        <v>13</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="3">
+        <v>14</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="40"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="6">
+        <v>15</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A22" s="40"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="6">
+        <v>16</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="40"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="6">
+        <v>17</v>
+      </c>
+      <c r="E23" s="42"/>
+      <c r="F23" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="43"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="9">
+        <v>18</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="45"/>
+      <c r="B25" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="48">
+        <v>19</v>
+      </c>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="50" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B20:B24"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="C7:C12"/>
     <mergeCell ref="B3:I5"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>